<commit_message>
adding matchday 6 data
</commit_message>
<xml_diff>
--- a/data/Bundesliga Filter Statistics.xlsx
+++ b/data/Bundesliga Filter Statistics.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3151"/>
+  <dimension ref="A1:H3169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
@@ -82415,6 +82415,474 @@
       </c>
       <c r="H3151" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3152">
+      <c r="A3152" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3152" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3152" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3152" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3152" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3152" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3152" t="n">
+        <v>21</v>
+      </c>
+      <c r="H3152" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3153">
+      <c r="A3153" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3153" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3153" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3153" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3153" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3153" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3153" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3153" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3154">
+      <c r="A3154" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3154" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3154" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3154" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3154" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3154" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3154" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3154" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3155">
+      <c r="A3155" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3155" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3155" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3155" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3155" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3155" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3155" t="n">
+        <v>25</v>
+      </c>
+      <c r="H3155" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3156">
+      <c r="A3156" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3156" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3156" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3156" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3156" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3156" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3156" t="n">
+        <v>17</v>
+      </c>
+      <c r="H3156" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3157">
+      <c r="A3157" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3157" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3157" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3157" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3157" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3157" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3157" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3157" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3158">
+      <c r="A3158" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3158" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3158" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3158" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3158" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3158" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3158" t="n">
+        <v>22</v>
+      </c>
+      <c r="H3158" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3159">
+      <c r="A3159" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3159" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3159" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3159" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3159" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3159" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3159" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3159" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3160">
+      <c r="A3160" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3160" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3160" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3160" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3160" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3160" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3160" t="n">
+        <v>11</v>
+      </c>
+      <c r="H3160" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3161">
+      <c r="A3161" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3161" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3161" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3161" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3161" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3161" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3161" t="n">
+        <v>23</v>
+      </c>
+      <c r="H3161" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3162">
+      <c r="A3162" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3162" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3162" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3162" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3162" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3162" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3162" t="n">
+        <v>16</v>
+      </c>
+      <c r="H3162" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3163">
+      <c r="A3163" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3163" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3163" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3163" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3163" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3163" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3163" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3163" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3164">
+      <c r="A3164" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3164" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3164" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3164" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3164" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3164" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3164" t="n">
+        <v>12</v>
+      </c>
+      <c r="H3164" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3165">
+      <c r="A3165" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3165" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3165" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3165" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3165" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3165" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3165" t="n">
+        <v>24</v>
+      </c>
+      <c r="H3165" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3166">
+      <c r="A3166" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3166" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3166" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3166" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3166" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3166" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3166" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3166" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3167">
+      <c r="A3167" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3167" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3167" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3167" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3167" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3167" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3167" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3168">
+      <c r="A3168" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3168" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3168" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3168" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3168" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3168" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3168" t="n">
+        <v>19</v>
+      </c>
+      <c r="H3168" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3169">
+      <c r="A3169" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3169" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3169" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3169" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3169" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3169" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3169" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3169" t="n">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>